<commit_message>
Sub array Sort with better time complexity.
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>Fibonacci Number</t>
   </si>
@@ -54,6 +54,21 @@
   </si>
   <si>
     <t>H-SubArraySort (Find the Minimum length Unsorted Subarray, sorting which makes the complete array sorted)</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key is to find min and max elements in the identified unsorted array. </t>
+  </si>
+  <si>
+    <t>Python Concepts</t>
+  </si>
+  <si>
+    <t>For decrement, For increment loop, break</t>
   </si>
 </sst>
 </file>
@@ -145,7 +160,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -155,6 +170,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -441,27 +459,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="40.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="1" max="4" width="40.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -475,47 +493,62 @@
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Analysis for Binary search
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Education\DataStructures\AlgoExpert\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chagag\Data\GitRepo\AlgoExpert\AlgoExpert\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561B94A7-7BAD-47D0-9A0B-7E9F6AD62E4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>Fibonacci Number</t>
   </si>
@@ -69,12 +70,27 @@
   </si>
   <si>
     <t>For decrement, For increment loop, break</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>Type conversion</t>
+  </si>
+  <si>
+    <t>We find mid element and compare it with target and based upon the comparision we reduce our search range.</t>
+  </si>
+  <si>
+    <t>O(log n)</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/binary-search/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -160,7 +176,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -175,6 +191,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -458,20 +479,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="40.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="1" max="4" width="40.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
@@ -500,7 +521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -526,7 +547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -549,14 +570,35 @@
         <v>4</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{4131A49F-42E2-4FB2-84A8-E34ACECC9619}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Binary search iteratively - Solution 2
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chagag\Data\GitRepo\AlgoExpert\AlgoExpert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561B94A7-7BAD-47D0-9A0B-7E9F6AD62E4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C18E9B3-FAC6-4042-9FBF-43FF5E814F11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,8 +24,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Gokul Chagalamarri Nippani</author>
+  </authors>
+  <commentList>
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{308D50D8-4D68-4D12-9B49-AD21BEF3893C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gokul Chagalamarri Nippani:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+If implemented recurresively because of stack.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{ECA80551-315A-474D-84C5-BF87A793A8D1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gokul Chagalamarri Nippani:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+If implemented iteratively</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>Fibonacci Number</t>
   </si>
@@ -85,13 +143,16 @@
   </si>
   <si>
     <t>https://www.geeksforgeeks.org/binary-search/</t>
+  </si>
+  <si>
+    <t>Problems</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +196,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -176,15 +250,12 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -479,20 +550,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="40.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="40.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="40.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
@@ -522,7 +599,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -548,16 +625,16 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -574,22 +651,28 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -600,5 +683,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Largest Range - Solution 1 (Can be done better)
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chagag\Data\GitRepo\AlgoExpert\AlgoExpert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C18E9B3-FAC6-4042-9FBF-43FF5E814F11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3C402F-7F25-4AD0-B52A-F0BE4CEF96FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,12 +78,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{D754C26C-ACEB-4DC0-8639-FDC061D9DE94}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gokul Chagalamarri Nippani:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+We will be accessing all the nodes.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{7912FC8F-436F-4BD5-93C8-938992351D32}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gokul Chagalamarri Nippani:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Call Stack. Where d is depth of tree.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Fibonacci Number</t>
   </si>
@@ -146,6 +194,30 @@
   </si>
   <si>
     <t>Problems</t>
+  </si>
+  <si>
+    <t>Vallidate BST</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/a-program-to-check-if-a-binary-tree-is-bst-or-not/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We need to compare each node value with max and min value </t>
+  </si>
+  <si>
+    <t>initialize max and min value</t>
+  </si>
+  <si>
+    <t>O(d)</t>
+  </si>
+  <si>
+    <t>Largrest Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O(1) </t>
+  </si>
+  <si>
+    <t>Solution 1: Make sure to compare current range with largest range before returning the result.</t>
   </si>
 </sst>
 </file>
@@ -250,23 +322,22 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -551,18 +622,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40.33203125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="40.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40.33203125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" style="7" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -570,10 +641,10 @@
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -602,7 +673,7 @@
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -628,13 +699,13 @@
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -654,7 +725,7 @@
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -674,15 +745,56 @@
       </c>
       <c r="H4" s="3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{4131A49F-42E2-4FB2-84A8-E34ACECC9619}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{3AC9589D-4F87-4092-A3B0-153341302977}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day 2: Array, DP
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u1d2pn\Algorithms\AlgoExpert\AlgoExpert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132A0488-EE8B-483E-80C9-AE626255868A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0679FF81-1E64-49A8-8D60-707427F3870E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Array" sheetId="2" r:id="rId2"/>
     <sheet name="Dynamic Programming" sheetId="3" r:id="rId3"/>
+    <sheet name="Linked List" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -133,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
   <si>
     <t>Fibonacci Number</t>
   </si>
@@ -234,13 +235,6 @@
     <t>array = [12, 3, 1, 2, -6, 5, -8, 6]          target = 0</t>
   </si>
   <si>
-    <t>Write a function that takes in a non-empty array of distinct integers and an integer representing a target sum. The function should find all triplets in
-  the array that sum up to the target sum and return a two-dimensional array of
-  all these triplets. The numbers in each triplet should be ordered in ascending
-  order, and the triplets themselves should be ordered in ascending order with
-  respect to the numbers they hold.</t>
-  </si>
-  <si>
     <t>O(n^2)</t>
   </si>
   <si>
@@ -278,6 +272,86 @@
   </si>
   <si>
     <t>O(nd)</t>
+  </si>
+  <si>
+    <t>Write a function that takes in a non-empty array of distinct integers and an integer representing a target sum. The function should find all triplets in the array that sum up to the target sum and return a two-dimensional array of all these triplets. The numbers in each triplet should be ordered in ascending order, and the triplets themselves should be ordered in ascending order with respect to the numbers they hold.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Num Sum </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[7, 6, 4, -1, 1, 2], target = 16 </t>
+  </si>
+  <si>
+    <t>[[6, 7, 1, 2], [6, 7, -1, 4]]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>extend</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ([6].extend([5] = [6, 5])),      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>append</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ([6].append([5] = [6, [5]]))</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Min Number of Coins For Change </t>
+  </si>
+  <si>
+    <t>n = 7, denoms = [1,5,10]</t>
+  </si>
+  <si>
+    <t>Given an array of positive integers representing coin denominations and a single non-negative integer representing a target amount of money, write a function that returns the smallest number of coins needed to make change for that target amount using the given coin denominations. If it's impossible to make change for the target amount, return -1</t>
+  </si>
+  <si>
+    <t>Average O(n^2) Worst O(n^3)</t>
+  </si>
+  <si>
+    <t>Levenshtein Distance</t>
+  </si>
+  <si>
+    <t>Write a function that takes in two strings and returns the minimum number of edit operations that need to be performed on the first string to obtain the second string.</t>
+  </si>
+  <si>
+    <t>str1 = = "abc", str2= "yabd"   (insert "y"; substitute "c" for "d")</t>
+  </si>
+  <si>
+    <t>O(nm)</t>
   </si>
 </sst>
 </file>
@@ -382,7 +456,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -400,9 +474,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
@@ -691,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -871,92 +942,111 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDF5E48-AA60-414B-B0B8-DF8AD2CBFD33}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="66.25" customWidth="1"/>
-    <col min="3" max="4" width="28.375" customWidth="1"/>
+    <col min="3" max="3" width="28.375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="28.375" customWidth="1"/>
+    <col min="5" max="5" width="14.75" style="9" customWidth="1"/>
     <col min="6" max="6" width="10.125" customWidth="1"/>
+    <col min="7" max="7" width="35.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="99.85" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" t="s">
-        <v>34</v>
-      </c>
       <c r="F3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
       <c r="B4" s="9"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
+      <c r="C5" s="8"/>
       <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -969,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E873AA64-7ED1-4CD6-BA39-733B4800E71A}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -980,6 +1070,7 @@
     <col min="1" max="1" width="31.125" customWidth="1"/>
     <col min="2" max="2" width="43.5" customWidth="1"/>
     <col min="3" max="3" width="24" style="9" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -990,10 +1081,10 @@
         <v>6</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="11" t="s">
         <v>36</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -1004,15 +1095,15 @@
     </row>
     <row r="2" spans="1:6" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2">
+      <c r="D2" s="9">
         <v>330</v>
       </c>
       <c r="E2" t="s">
@@ -1024,22 +1115,110 @@
     </row>
     <row r="3" spans="1:6" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="9">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
         <v>45</v>
       </c>
-      <c r="D3">
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="114.15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="9">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="9">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
+      <c r="E5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;8&amp;K000000Sensitivity: General/Internal</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEFE5C12-E91A-4E0A-91C0-8D6DB04B20A7}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="3" max="3" width="30" style="9" customWidth="1"/>
+    <col min="4" max="4" width="14.875" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day 3 - BST, Search, String and Stacks
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u1d2pn\Algorithms\AlgoExpert\AlgoExpert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0679FF81-1E64-49A8-8D60-707427F3870E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C45742E-36FB-4629-AAE3-422FE410260A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Array" sheetId="2" r:id="rId2"/>
     <sheet name="Dynamic Programming" sheetId="3" r:id="rId3"/>
-    <sheet name="Linked List" sheetId="4" r:id="rId4"/>
+    <sheet name="BinarySearchTrees" sheetId="5" r:id="rId4"/>
+    <sheet name="Linked List" sheetId="4" r:id="rId5"/>
+    <sheet name="Searching" sheetId="7" r:id="rId6"/>
+    <sheet name="Strings" sheetId="6" r:id="rId7"/>
+    <sheet name="Stacks" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -134,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="71">
   <si>
     <t>Fibonacci Number</t>
   </si>
@@ -352,6 +356,165 @@
   </si>
   <si>
     <t>O(nm)</t>
+  </si>
+  <si>
+    <t>Find Closest Value In BST</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Average</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: O(log(n))    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Worst</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: O(n) - If only one branch</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Iterative Solution </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">We will have stack frame Average: O(log(n))    Worst: O(n) - If only one branch                     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Recursive Solution  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Worst: O(1)</t>
+    </r>
+  </si>
+  <si>
+    <t>abs- absolute value           float("inf")- Max value</t>
+  </si>
+  <si>
+    <t>Array -[0, 1, 21, 33, 45, 45, 61, 71, 72, 73]    target:33</t>
+  </si>
+  <si>
+    <t>O(logn)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Recurssive: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">O(log(n)) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Iterative: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>O(1)</t>
+    </r>
+  </si>
+  <si>
+    <t>Palindrome Check</t>
+  </si>
+  <si>
+    <t>"abcdcba"</t>
+  </si>
+  <si>
+    <t>Write a function that takes in a non-empty string and that returns a boolean representing whether the string is a palindrome.</t>
+  </si>
+  <si>
+    <t>Min Max Stack Construction</t>
+  </si>
+  <si>
+    <t>Get min and max value in a stack in O(1) time</t>
   </si>
 </sst>
 </file>
@@ -495,6 +658,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>250165</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>43131</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1388852</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1262269</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05F4B502-BEE7-4B00-BA6E-E903215A1FF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3838754" y="224286"/>
+          <a:ext cx="1138687" cy="1219138"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -762,7 +980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -945,7 +1163,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1062,7 +1280,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1183,6 +1401,74 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DACDE2C-02E0-4EB1-B18E-F685A530C42A}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.375" customWidth="1"/>
+    <col min="2" max="2" width="23.625" customWidth="1"/>
+    <col min="3" max="3" width="23.375" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="9" customWidth="1"/>
+    <col min="6" max="6" width="19.625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="29.375" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2">
+        <v>13</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;8&amp;K000000Sensitivity: General/Internal</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEFE5C12-E91A-4E0A-91C0-8D6DB04B20A7}">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -1228,4 +1514,203 @@
     <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;8&amp;K000000Sensitivity: General/Internal</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468127C9-FF2E-443C-A022-9FA58D692751}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.125" customWidth="1"/>
+    <col min="2" max="2" width="16.375" customWidth="1"/>
+    <col min="3" max="3" width="36.875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="11.75" customWidth="1"/>
+    <col min="6" max="6" width="22.625" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;8&amp;K000000Sensitivity: General/Internal</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA983656-2E0C-400C-B523-0A09A33AE010}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.375" customWidth="1"/>
+    <col min="2" max="2" width="27.875" customWidth="1"/>
+    <col min="3" max="3" width="17.125" customWidth="1"/>
+    <col min="4" max="4" width="14.625" customWidth="1"/>
+    <col min="5" max="5" width="12.875" customWidth="1"/>
+    <col min="7" max="7" width="21.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;8&amp;K000000Sensitivity: General/Internal</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE3994E-1DB6-498F-AD7A-DC81053B32B0}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.875" customWidth="1"/>
+    <col min="2" max="2" width="48.875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="18.125" customWidth="1"/>
+    <col min="4" max="4" width="11.75" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="14.75" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;8&amp;K000000Sensitivity: General/Internal</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Day 4: bst constuction, invert bst, remove kth node from end, nth fib
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u1d2pn\Algorithms\AlgoExpert\AlgoExpert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C45742E-36FB-4629-AAE3-422FE410260A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D15F0A-31FF-4DE5-B56D-CE447F92D27E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,11 @@
     <sheet name="Searching" sheetId="7" r:id="rId6"/>
     <sheet name="Strings" sheetId="6" r:id="rId7"/>
     <sheet name="Stacks" sheetId="8" r:id="rId8"/>
+    <sheet name="BinaryTrees" sheetId="9" r:id="rId9"/>
+    <sheet name="Recursion" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -138,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="84">
   <si>
     <t>Fibonacci Number</t>
   </si>
@@ -515,6 +518,45 @@
   </si>
   <si>
     <t>Get min and max value in a stack in O(1) time</t>
+  </si>
+  <si>
+    <t>BST Construction</t>
+  </si>
+  <si>
+    <t>Insert, Delete, Contain</t>
+  </si>
+  <si>
+    <t>I/C/D: O(log(n)) , O(n)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I/C/D: O(1) , O(n)    </t>
+  </si>
+  <si>
+    <t>Invert Binary Tree</t>
+  </si>
+  <si>
+    <t>Swap a and b: a,b = b,a</t>
+  </si>
+  <si>
+    <t>Iterative : O(n)      Recursive: O(d)</t>
+  </si>
+  <si>
+    <t>Nth Fibonacci</t>
+  </si>
+  <si>
+    <t>fib series is 0,1,1,2,3,5,8</t>
+  </si>
+  <si>
+    <t>Remove Kth Node From End</t>
+  </si>
+  <si>
+    <t>Write a function that takes in the head of a Singly Linked List and an integer and removes the kth node from the end of the list.</t>
+  </si>
+  <si>
+    <t>0 -&gt; 1 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 6 -&gt; 7 -&gt; 8 -&gt; 9  k=4</t>
+  </si>
+  <si>
+    <t>0 -&gt; 1 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 7 -&gt; 8 -&gt; 9</t>
   </si>
 </sst>
 </file>
@@ -1158,6 +1200,75 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787C0BAA-16C9-4B16-9224-02568B13CFFE}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.875" customWidth="1"/>
+    <col min="2" max="2" width="23.25" customWidth="1"/>
+    <col min="4" max="4" width="13.25" customWidth="1"/>
+    <col min="5" max="5" width="14.75" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;8&amp;K000000Sensitivity: General/Internal</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDF5E48-AA60-414B-B0B8-DF8AD2CBFD33}">
   <dimension ref="A1:G5"/>
@@ -1402,10 +1513,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DACDE2C-02E0-4EB1-B18E-F685A530C42A}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1413,7 +1524,7 @@
     <col min="1" max="1" width="28.375" customWidth="1"/>
     <col min="2" max="2" width="23.625" customWidth="1"/>
     <col min="3" max="3" width="23.375" customWidth="1"/>
-    <col min="5" max="5" width="16.5" style="9" customWidth="1"/>
+    <col min="5" max="5" width="22.75" style="9" customWidth="1"/>
     <col min="6" max="6" width="19.625" style="9" customWidth="1"/>
     <col min="7" max="7" width="29.375" style="9" customWidth="1"/>
   </cols>
@@ -1456,6 +1567,20 @@
       </c>
       <c r="G2" s="9" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1470,18 +1595,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEFE5C12-E91A-4E0A-91C0-8D6DB04B20A7}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="2" max="2" width="45.5" style="9" customWidth="1"/>
     <col min="3" max="3" width="30" style="9" customWidth="1"/>
-    <col min="4" max="4" width="14.875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="22.125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="13.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1505,6 +1631,26 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1654,7 +1800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE3994E-1DB6-498F-AD7A-DC81053B32B0}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -1713,4 +1859,68 @@
     <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;8&amp;K000000Sensitivity: General/Internal</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C6B7BC-132E-4AAE-901D-1BBC3D3394F6}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.375" customWidth="1"/>
+    <col min="2" max="2" width="16.75" customWidth="1"/>
+    <col min="3" max="3" width="13.125" customWidth="1"/>
+    <col min="4" max="5" width="12.25" customWidth="1"/>
+    <col min="6" max="6" width="20.25" style="9" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;8&amp;K000000Sensitivity: General/Internal</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Day 5 - Smallest Diff, sub array sort, max increasing sub seq, max sum increasing seq
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u1d2pn\Algorithms\AlgoExpert\AlgoExpert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D15F0A-31FF-4DE5-B56D-CE447F92D27E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B7FCC1-CBA0-4503-B52C-498231ADF07D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
     <sheet name="Recursion" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -141,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="103">
   <si>
     <t>Fibonacci Number</t>
   </si>
@@ -355,9 +354,6 @@
     <t>Write a function that takes in two strings and returns the minimum number of edit operations that need to be performed on the first string to obtain the second string.</t>
   </si>
   <si>
-    <t>str1 = = "abc", str2= "yabd"   (insert "y"; substitute "c" for "d")</t>
-  </si>
-  <si>
     <t>O(nm)</t>
   </si>
   <si>
@@ -557,6 +553,66 @@
   </si>
   <si>
     <t>0 -&gt; 1 -&gt; 2 -&gt; 3 -&gt; 4 -&gt; 5 -&gt; 7 -&gt; 8 -&gt; 9</t>
+  </si>
+  <si>
+    <t>Smallest Difference</t>
+  </si>
+  <si>
+    <t>Write a function that takes in two non-empty arrays of integers, finds the pair of numbers (one from each array) whose absolute difference is closest to zero, and returns an array containing these two numbers, with the number from the first array in the first position.</t>
+  </si>
+  <si>
+    <t>array1 = [-1, 5, 10, 20, 28, 3]     array2 = [26, 134, 135, 15, 17]</t>
+  </si>
+  <si>
+    <t>[28, 26]</t>
+  </si>
+  <si>
+    <t>O(nlog(n)) + O(mlog(m)</t>
+  </si>
+  <si>
+    <t>Subarray Sort</t>
+  </si>
+  <si>
+    <t>Write a function that takes in an array of at least two integers and that returns an array of the starting and ending indices of the smallest subarray in the input array that needs to be sorted in place in order for the entire input array to be sorted.  If the input array is already sorted, the function should return [-1,-1]</t>
+  </si>
+  <si>
+    <t>[1, 2, 4, 7, 10, 11, 7, 12, 6, 7, 16, 18, 19]</t>
+  </si>
+  <si>
+    <t>[3, 9]</t>
+  </si>
+  <si>
+    <t>Max Sum Increasing Subsequence</t>
+  </si>
+  <si>
+    <t>Write a function that takes in a non-empty array of integers and returns the greatest sum that can be generated from a strictly-increasing subsequence in the array as well as an array of the numbers in that subsequence. You can assume that there will only be one increasing subsequence with the greatest sum.</t>
+  </si>
+  <si>
+    <t>[10, 70, 20, 30, 50, 11, 30]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[110, [10, 20, 30, 50]] </t>
+  </si>
+  <si>
+    <t>Longest Common Subsequence</t>
+  </si>
+  <si>
+    <t>Write a function that takes in two strings and returns their longest common subsequence.</t>
+  </si>
+  <si>
+    <t>["X", "Y", "Z", "W"]</t>
+  </si>
+  <si>
+    <t>str11 = "ZXVVYZW" str2 = "XKYKZPW"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">str1 = = "abc", str2= "yabd"   (insert "y"; substitute "c" for "d") </t>
+  </si>
+  <si>
+    <t>2D array:  [[i for i in range(len(str1)+1)] for i in range(len(str2)+1)]</t>
+  </si>
+  <si>
+    <t>2D array with all zeros: [[0 for x in range(len(str2)+1)] for x in range(len(str1)+1)]</t>
   </si>
 </sst>
 </file>
@@ -1242,10 +1298,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
         <v>78</v>
-      </c>
-      <c r="B2" t="s">
-        <v>79</v>
       </c>
       <c r="C2">
         <v>6</v>
@@ -1271,17 +1327,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDF5E48-AA60-414B-B0B8-DF8AD2CBFD33}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="66.25" customWidth="1"/>
-    <col min="3" max="3" width="28.375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="34.25" style="7" customWidth="1"/>
     <col min="4" max="4" width="28.375" customWidth="1"/>
     <col min="5" max="5" width="14.75" style="9" customWidth="1"/>
     <col min="6" max="6" width="10.125" customWidth="1"/>
@@ -1372,10 +1428,45 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="9"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
+    <row r="5" spans="1:7" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1388,10 +1479,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E873AA64-7ED1-4CD6-BA39-733B4800E71A}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1399,10 +1490,11 @@
     <col min="1" max="1" width="31.125" customWidth="1"/>
     <col min="2" max="2" width="43.5" customWidth="1"/>
     <col min="3" max="3" width="24" style="9" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="9" customWidth="1"/>
+    <col min="4" max="4" width="18.125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="47.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1421,8 +1513,11 @@
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -1442,7 +1537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="57.1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1462,7 +1557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="114.15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="114.15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1482,7 +1577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="57.1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1490,16 +1585,56 @@
         <v>56</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="D5" s="9">
         <v>2</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="99.85" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1554,33 +1689,33 @@
     </row>
     <row r="2" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2">
         <v>13</v>
       </c>
       <c r="E2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
         <v>71</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1597,7 +1732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEFE5C12-E91A-4E0A-91C0-8D6DB04B20A7}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1635,16 +1770,16 @@
     </row>
     <row r="2" spans="1:7" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>82</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>83</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>4</v>
@@ -1705,16 +1840,16 @@
         <v>15</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1769,13 +1904,13 @@
     </row>
     <row r="2" spans="1:7" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
         <v>66</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" t="s">
-        <v>67</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1840,10 +1975,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>70</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
@@ -1904,16 +2039,16 @@
     </row>
     <row r="2" spans="1:7" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day 6: Min Heap Construction, DFS, Caesar Cipher Encryptor
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u1d2pn\Algorithms\AlgoExpert\AlgoExpert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B7FCC1-CBA0-4503-B52C-498231ADF07D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977DDCD8-C2B0-41E6-B2AA-C489C2AF8360}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,11 @@
     <sheet name="Linked List" sheetId="4" r:id="rId5"/>
     <sheet name="Searching" sheetId="7" r:id="rId6"/>
     <sheet name="Strings" sheetId="6" r:id="rId7"/>
-    <sheet name="Stacks" sheetId="8" r:id="rId8"/>
-    <sheet name="BinaryTrees" sheetId="9" r:id="rId9"/>
-    <sheet name="Recursion" sheetId="10" r:id="rId10"/>
+    <sheet name="Heaps" sheetId="11" r:id="rId8"/>
+    <sheet name="Graphs" sheetId="12" r:id="rId9"/>
+    <sheet name="Stacks" sheetId="8" r:id="rId10"/>
+    <sheet name="Recursion" sheetId="10" r:id="rId11"/>
+    <sheet name="BinaryTrees" sheetId="9" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -140,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="116">
   <si>
     <t>Fibonacci Number</t>
   </si>
@@ -613,6 +615,68 @@
   </si>
   <si>
     <t>2D array with all zeros: [[0 for x in range(len(str2)+1)] for x in range(len(str1)+1)]</t>
+  </si>
+  <si>
+    <t>The space complexity can be improved.</t>
+  </si>
+  <si>
+    <t>Min Heap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peek O(1) BuildHeap - O(n)  SiftDown/SiftUp/Insert/Remove - O(log(n))  </t>
+  </si>
+  <si>
+    <t>All - O(1)</t>
+  </si>
+  <si>
+    <t>Depth First Search</t>
+  </si>
+  <si>
+    <t>O(v+e)</t>
+  </si>
+  <si>
+    <t>O(v)</t>
+  </si>
+  <si>
+    <t>Caesar Cipher Encryptor</t>
+  </si>
+  <si>
+    <t>Given a non-empty string of lowercase letters and a non-negative integer representing a key, write a function that returns a new string obtained by shifting every letter in the input string by k positions in the alphabet, where k is the key.</t>
+  </si>
+  <si>
+    <t>str = "xyz", k=2</t>
+  </si>
+  <si>
+    <t>"zab"</t>
+  </si>
+  <si>
+    <t>ord('a') = 97 ; chr(97) = 'a'  list("abc") = ['a','b','c']</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Decrementing For loop: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>for i in reversed(range(6)):</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1079,7 +1143,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1257,6 +1321,71 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE3994E-1DB6-498F-AD7A-DC81053B32B0}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.875" customWidth="1"/>
+    <col min="2" max="2" width="48.875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="18.125" customWidth="1"/>
+    <col min="4" max="4" width="11.75" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="14.75" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;8&amp;K000000Sensitivity: General/Internal</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787C0BAA-16C9-4B16-9224-02568B13CFFE}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1325,12 +1454,76 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C6B7BC-132E-4AAE-901D-1BBC3D3394F6}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.375" customWidth="1"/>
+    <col min="2" max="2" width="16.75" customWidth="1"/>
+    <col min="3" max="3" width="13.125" customWidth="1"/>
+    <col min="4" max="5" width="12.25" customWidth="1"/>
+    <col min="6" max="6" width="20.25" style="9" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;8&amp;K000000Sensitivity: General/Internal</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDF5E48-AA60-414B-B0B8-DF8AD2CBFD33}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1479,10 +1672,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E873AA64-7ED1-4CD6-BA39-733B4800E71A}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1492,9 +1685,10 @@
     <col min="3" max="3" width="24" style="9" customWidth="1"/>
     <col min="4" max="4" width="18.125" style="9" customWidth="1"/>
     <col min="7" max="7" width="47.375" customWidth="1"/>
+    <col min="8" max="8" width="32.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1517,7 +1711,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -1537,7 +1731,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="57.1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1557,7 +1751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="114.15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="114.15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1577,7 +1771,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="57.1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1599,8 +1793,11 @@
       <c r="G5" s="9" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="99.85" x14ac:dyDescent="0.25">
+      <c r="H5" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="99.85" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>92</v>
       </c>
@@ -1620,7 +1817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -1632,6 +1829,12 @@
       </c>
       <c r="D7" s="9" t="s">
         <v>98</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>102</v>
@@ -1651,7 +1854,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1802,7 +2005,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1863,10 +2066,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA983656-2E0C-400C-B523-0A09A33AE010}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1876,7 +2079,7 @@
     <col min="3" max="3" width="17.125" customWidth="1"/>
     <col min="4" max="4" width="14.625" customWidth="1"/>
     <col min="5" max="5" width="12.875" customWidth="1"/>
-    <col min="7" max="7" width="21.25" customWidth="1"/>
+    <col min="7" max="7" width="30.75" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1920,6 +2123,29 @@
       </c>
       <c r="F2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="114.15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1932,22 +2158,22 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE3994E-1DB6-498F-AD7A-DC81053B32B0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C7AEC2-EDD1-4464-BCC2-63EA07DB7B5B}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.875" customWidth="1"/>
-    <col min="2" max="2" width="48.875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="18.125" customWidth="1"/>
-    <col min="4" max="4" width="11.75" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="14.75" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="1" max="1" width="23.625" customWidth="1"/>
+    <col min="2" max="2" width="34.375" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="23" style="9" customWidth="1"/>
+    <col min="6" max="6" width="24" style="9" customWidth="1"/>
+    <col min="7" max="7" width="34.875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1957,34 +2183,34 @@
       <c r="B1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
+        <v>104</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1997,21 +2223,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C6B7BC-132E-4AAE-901D-1BBC3D3394F6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ECC95F4-0C1B-4B84-A2B6-50E32685C38B}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.375" customWidth="1"/>
-    <col min="2" max="2" width="16.75" customWidth="1"/>
-    <col min="3" max="3" width="13.125" customWidth="1"/>
-    <col min="4" max="5" width="12.25" customWidth="1"/>
-    <col min="6" max="6" width="20.25" style="9" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="13.25" customWidth="1"/>
+    <col min="7" max="7" width="22.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2021,13 +2247,13 @@
       <c r="B1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="5" t="s">
@@ -2037,18 +2263,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G2" t="s">
-        <v>75</v>
+        <v>108</v>
+      </c>
+      <c r="F2" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>